<commit_message>
Setup PyQt5 for GUI Development
Signed-off-by: Saurabh Prakash <saurabhprakash.smvit@gmail.com>
</commit_message>
<xml_diff>
--- a/weight_monitoring.xlsx
+++ b/weight_monitoring.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - Tally Solutions Pvt. Ltd\desktop\Personal\Weight Graph\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - Tally Solutions Pvt. Ltd\desktop\Personal\Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{075342E5-F39B-472E-A532-EB2213DF76BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED6B966-B538-4A9B-8295-CFA1BE0F827E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -357,16 +357,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.36328125" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -377,459 +377,732 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43863</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B2">
+        <v>109.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43864</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43865</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43866</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43867</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43868</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43869</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43870</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43871</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43872</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43873</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43874</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43875</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43876</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43877</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43878</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43879</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43880</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43881</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43882</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43883</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43884</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43885</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43886</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43887</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43888</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43889</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43890</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>43891</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>43892</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>43893</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>43894</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>43895</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>43896</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>43897</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>43898</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>43899</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>43900</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>43901</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>43902</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>43903</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43904</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43905</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43906</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>43907</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>43908</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>43909</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>43910</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>43911</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>43912</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>43913</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>43914</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>43915</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>43916</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>43917</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>43918</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>43919</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>43920</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>43921</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>43922</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>43923</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>43924</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>43925</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>43926</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>43927</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>43928</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>43929</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>43930</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>43931</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>43932</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>43933</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>43934</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>43935</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>43936</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>43937</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>43938</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>43939</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>43940</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>43941</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>43942</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>43943</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>43944</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>43945</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>43946</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>43947</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>43948</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>43949</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>43950</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>43951</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>43952</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>43953</v>
+      </c>
+      <c r="B92">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make a QDOubleSpinBox widget that shows the slider value
Signed-off-by: Saurabh Prakash <saurabhprakash.smvit@gmail.com>
</commit_message>
<xml_diff>
--- a/weight_monitoring.xlsx
+++ b/weight_monitoring.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - Tally Solutions Pvt. Ltd\desktop\Personal\Tracker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saurabh.prakash\PycharmProjects\Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED6B966-B538-4A9B-8295-CFA1BE0F827E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3546E65B-291C-405C-9BB7-9F2877A55CCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -357,8 +357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="D92" sqref="D92"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -390,7 +390,7 @@
         <v>43864</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>110.4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>